<commit_message>
Added ExcelObject class to create JSON objects later
</commit_message>
<xml_diff>
--- a/Resources/sampledata.xlsx
+++ b/Resources/sampledata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\livieric\Documents\GitHub Projects\visualdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\livieric\Documents\GitHub Projects\visualdata\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,42 +24,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
-  <si>
-    <t>pages</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>author</t>
-  </si>
-  <si>
-    <t>hickory</t>
-  </si>
-  <si>
-    <t>green</t>
-  </si>
-  <si>
-    <t>banana</t>
-  </si>
-  <si>
-    <t>timber</t>
-  </si>
-  <si>
-    <t>freebird</t>
-  </si>
-  <si>
-    <t>boo</t>
-  </si>
-  <si>
-    <t>ann</t>
-  </si>
-  <si>
-    <t>joe</t>
-  </si>
-  <si>
-    <t>bob</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Naboo</t>
+  </si>
+  <si>
+    <t>Alderaan</t>
+  </si>
+  <si>
+    <t>Tatooine</t>
+  </si>
+  <si>
+    <t>Coruscant</t>
   </si>
 </sst>
 </file>
@@ -95,8 +77,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,89 +360,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="1">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>732</v>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5000000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <v>346</v>
+      <c r="B5" s="1">
+        <v>10000000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated with graph processing rows properly
</commit_message>
<xml_diff>
--- a/Resources/sampledata.xlsx
+++ b/Resources/sampledata.xlsx
@@ -29,19 +29,19 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Population</t>
-  </si>
-  <si>
-    <t>Naboo</t>
-  </si>
-  <si>
-    <t>Alderaan</t>
-  </si>
-  <si>
-    <t>Tatooine</t>
-  </si>
-  <si>
-    <t>Coruscant</t>
+    <t>Price per ft^2</t>
+  </si>
+  <si>
+    <t>San Francisco, CA</t>
+  </si>
+  <si>
+    <t>Belhaven, NC</t>
+  </si>
+  <si>
+    <t>Dallas, TX</t>
+  </si>
+  <si>
+    <t>New York City, NY</t>
   </si>
 </sst>
 </file>
@@ -363,12 +363,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="17.88671875" customWidth="1"/>
   </cols>
@@ -386,7 +386,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>1000000</v>
+        <v>728</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -394,7 +394,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -402,7 +402,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>5000000</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -410,7 +410,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>10000000000</v>
+        <v>650</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
number of data points function working
</commit_message>
<xml_diff>
--- a/Resources/sampledata.xlsx
+++ b/Resources/sampledata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25920" windowHeight="14688"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25920" windowHeight="14690"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Price per ft^2</t>
-  </si>
-  <si>
     <t>San Francisco, CA</t>
   </si>
   <si>
@@ -42,6 +36,12 @@
   </si>
   <si>
     <t>New York City, NY</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>price</t>
   </si>
 </sst>
 </file>
@@ -363,51 +363,51 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.6328125" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>728</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>650</v>

</xml_diff>

<commit_message>
Fix positioning to center
</commit_message>
<xml_diff>
--- a/Resources/sampledata.xlsx
+++ b/Resources/sampledata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\livieric\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\livieric\Documents\GitHub Projects\visualdata\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Location</t>
   </si>
@@ -41,7 +41,13 @@
     <t>New York City, NY</t>
   </si>
   <si>
-    <t>price</t>
+    <t xml:space="preserve">Price per Sq. Ft. </t>
+  </si>
+  <si>
+    <t>Philadelphia, PA</t>
+  </si>
+  <si>
+    <t>Denver, CO</t>
   </si>
 </sst>
 </file>
@@ -360,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -386,7 +392,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>728</v>
+        <v>847</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -410,7 +416,23 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>650</v>
+        <v>585</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data with real values
</commit_message>
<xml_diff>
--- a/Resources/sampledata.xlsx
+++ b/Resources/sampledata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\livieric\Documents\GitHub Projects\visualdata\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Livi\Documents\GitHub\visualdata\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -179,6 +179,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -214,6 +231,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -369,7 +403,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -392,7 +426,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>847</v>
+        <v>785</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -400,7 +434,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>28</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -408,7 +442,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -416,7 +450,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>585</v>
+        <v>446</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -424,7 +458,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -432,7 +466,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1">
-        <v>289</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>